<commit_message>
menu pemantauan dan benerin fitur2 ...selesai
</commit_message>
<xml_diff>
--- a/public/Template_Excel/penanganan_risiko.xlsx
+++ b/public/Template_Excel/penanganan_risiko.xlsx
@@ -16,47 +16,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+  <si>
+    <t>Triwulan I</t>
+  </si>
+  <si>
+    <t>Semester I</t>
+  </si>
+  <si>
+    <t>ID Penilaian Risiko</t>
+  </si>
+  <si>
+    <t>Opsi Penanganan
+Risiko SPBE (sesuaikan penulisan dengan daftar)</t>
+  </si>
   <si>
     <t>Rencana Aksi Penanganan Risiko SPBE</t>
   </si>
   <si>
     <t>Keluaran</t>
+  </si>
+  <si>
+    <t>Jenis Periode Implementasi</t>
   </si>
   <si>
     <t>Penanggung
 Jawab</t>
   </si>
   <si>
-    <t>Penyusunan surat edaran tentang prosedur pengiriman data sensus survey</t>
-  </si>
-  <si>
-    <t>Surat edaran tentang prosedur pengiriman data sensus survey</t>
-  </si>
-  <si>
-    <t>Direktur SIS</t>
-  </si>
-  <si>
-    <t>YA</t>
-  </si>
-  <si>
     <t>Apakah Terdapat Risiko
 Residual? (YA/TIDAK)</t>
   </si>
   <si>
-    <t>ID Penilaian Risiko</t>
-  </si>
-  <si>
-    <t>ID_11</t>
-  </si>
-  <si>
-    <t>Jadwal Selesai Implementasi (yyyy-mm-dd)</t>
-  </si>
-  <si>
-    <t>Jadwal Mulai Implementasi (yyyy-mm-dd)</t>
+    <t>ID_2</t>
   </si>
   <si>
     <t>Ekskalasi Risiko</t>
+  </si>
+  <si>
+    <t>Penyusunan surat edaran tentang prosedur pengiriman data sensus survey</t>
+  </si>
+  <si>
+    <t>Surat edaran tentang prosedur pengiriman data sensus survey</t>
+  </si>
+  <si>
+    <t>Triwulan</t>
+  </si>
+  <si>
+    <t>Direktur SIS</t>
+  </si>
+  <si>
+    <t>YA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Periode Implementasi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Jika "Jenis Periode Implementasi"-nya "Tanggal", maka kosongi)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tanggal Mulai Implementasi (yyyy-mm-dd)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Isi jika "Jenis Periode Implementasinya" -nya "Tanggal")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tanggal Selesai Implementasi (yyyy-mm-dd)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Isi jika "Jenis Periode Implementasinya" -nya "Tanggal")</t>
+    </r>
+  </si>
+  <si>
+    <t>Tanggal</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Januari</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>ID_3</t>
+  </si>
+  <si>
+    <t>ID_4</t>
+  </si>
+  <si>
+    <t>ID_5</t>
   </si>
   <si>
     <r>
@@ -127,8 +203,31 @@
     </r>
   </si>
   <si>
-    <t>Opsi Penanganan
-Risiko SPBE (sesuaikan penulisan dengan daftar)</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jenis Periode Implementasi:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Tanggal
+- Triwulan
+- Semester
+- Bulan</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -138,7 +237,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +279,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -201,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -291,43 +405,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -631,82 +781,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:10" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="5" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="13">
+        <v>44559</v>
+      </c>
+      <c r="H5" s="13">
+        <v>44581</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7">
-        <v>44559</v>
-      </c>
-      <c r="F4" s="7">
-        <v>44581</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>6</v>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>